<commit_message>
adds xmodem testing system
</commit_message>
<xml_diff>
--- a/flight-computer-pin-assignment-version-1.xlsx
+++ b/flight-computer-pin-assignment-version-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5th-year\project\N4-Flight-Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52288CD1-DA54-403E-A83E-A53944E97BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46833601-511F-4A76-8063-4DF316A6D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="0" windowWidth="17985" windowHeight="13050" xr2:uid="{C1B70286-B989-4919-B8D9-1F40D54E6E76}"/>
+    <workbookView xWindow="10305" yWindow="495" windowWidth="11925" windowHeight="12405" xr2:uid="{C1B70286-B989-4919-B8D9-1F40D54E6E76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t xml:space="preserve">N4 FLIGHT COMPUTER HARDWARE PIN ASSIGNMENT </t>
   </si>
@@ -72,15 +72,9 @@
     <t>Ground</t>
   </si>
   <si>
-    <t>PYRO1</t>
-  </si>
-  <si>
     <t>GPIO_25</t>
   </si>
   <si>
-    <t>PYRO2</t>
-  </si>
-  <si>
     <t>GPIO_12</t>
   </si>
   <si>
@@ -235,13 +229,28 @@
   </si>
   <si>
     <t>SD card chip select pin</t>
+  </si>
+  <si>
+    <t>DROGUE_PYRO</t>
+  </si>
+  <si>
+    <t>MAIN_PYRO</t>
+  </si>
+  <si>
+    <t>flash_led_pin</t>
+  </si>
+  <si>
+    <t>Blinks when formating onboard flash memory</t>
+  </si>
+  <si>
+    <t>GPIO_39</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +273,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -273,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -333,30 +348,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -368,6 +384,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56767EC-775B-46A7-97A3-9068651156DE}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,421 +727,432 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="4">
         <v>1</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="4">
         <v>2</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="4">
         <v>3</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="4">
         <v>4</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>5</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="D17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>7</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>11</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>13</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>15</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>16</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>17</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="B33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>18</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="B34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>6</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="B35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>20</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>21</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="B37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>22</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>7</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>8</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>9</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>10</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>11</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>12</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>13</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>14</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
-        <v>15</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>16</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
-        <v>17</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
-        <v>18</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
-        <v>19</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
-        <v>20</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
-        <v>21</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>69</v>
+      <c r="B38" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:F2"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A4:F5"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixes GPIO input bug :bug:
</commit_message>
<xml_diff>
--- a/flight-computer-pin-assignment-version-1.xlsx
+++ b/flight-computer-pin-assignment-version-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\5th-year\project\N4-Flight-Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46833601-511F-4A76-8063-4DF316A6D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25662C86-529C-44F5-8C22-486A599FC5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10305" yWindow="495" windowWidth="11925" windowHeight="12405" xr2:uid="{C1B70286-B989-4919-B8D9-1F40D54E6E76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
   <si>
     <t xml:space="preserve">N4 FLIGHT COMPUTER HARDWARE PIN ASSIGNMENT </t>
   </si>
@@ -243,7 +243,25 @@
     <t>Blinks when formating onboard flash memory</t>
   </si>
   <si>
-    <t>GPIO_39</t>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>INPUT/OUTPUT</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>CLOCK</t>
+  </si>
+  <si>
+    <t>GPIO_32</t>
   </si>
 </sst>
 </file>
@@ -363,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -376,6 +394,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -385,9 +410,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -395,9 +417,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,9 +731,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56767EC-775B-46A7-97A3-9068651156DE}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -722,101 +741,109 @@
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="3" max="4" width="32.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="1"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
         <v>5</v>
@@ -825,10 +852,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -839,10 +869,13 @@
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -853,10 +886,13 @@
         <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>3</v>
       </c>
@@ -867,10 +903,13 @@
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>4</v>
       </c>
@@ -881,10 +920,13 @@
         <v>15</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>5</v>
       </c>
@@ -895,10 +937,13 @@
         <v>16</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>6</v>
       </c>
@@ -909,10 +954,13 @@
         <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>7</v>
       </c>
@@ -923,10 +971,13 @@
         <v>23</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>8</v>
       </c>
@@ -937,10 +988,13 @@
         <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>9</v>
       </c>
@@ -951,10 +1005,13 @@
         <v>29</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>10</v>
       </c>
@@ -965,10 +1022,13 @@
         <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>11</v>
       </c>
@@ -979,10 +1039,13 @@
         <v>35</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>12</v>
       </c>
@@ -993,10 +1056,13 @@
         <v>38</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>13</v>
       </c>
@@ -1007,10 +1073,13 @@
         <v>41</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>14</v>
       </c>
@@ -1021,19 +1090,23 @@
         <v>44</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>15</v>
       </c>
@@ -1044,10 +1117,13 @@
         <v>48</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>16</v>
       </c>
@@ -1058,10 +1134,13 @@
         <v>51</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>17</v>
       </c>
@@ -1072,10 +1151,13 @@
         <v>54</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>18</v>
       </c>
@@ -1086,10 +1168,13 @@
         <v>57</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>19</v>
       </c>
@@ -1100,10 +1185,13 @@
         <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>20</v>
       </c>
@@ -1114,10 +1202,13 @@
         <v>63</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>21</v>
       </c>
@@ -1128,31 +1219,37 @@
         <v>66</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
         <v>22</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A4:F5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A4:G5"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>